<commit_message>
Add: All Gemini Quixbugs
</commit_message>
<xml_diff>
--- a/Analysis/QuixBugs_Gemini-APR/APR_one_shot_Gemini_1.0_Pro_Java.xlsx
+++ b/Analysis/QuixBugs_Gemini-APR/APR_one_shot_Gemini_1.0_Pro_Java.xlsx
@@ -8,14 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mraee\Desktop\Investigation\Bug Busters\Analysis\QuixBugs_Gemini-APR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{216E62CE-C130-46B6-90A2-A7B88145CD0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0F7275B-A6F1-4B2D-B5F1-6D5FFFF94898}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9480" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{17CD3759-C701-4D9B-B6BE-DFDE4B53E133}"/>
   </bookViews>
   <sheets>
     <sheet name="APR_one_shot_Gemini_1.0_Pro_Jav" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -5888,13 +5901,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7C37FC4-7C8D-4B7A-AFA1-7020484B2FBF}">
   <dimension ref="A1:J46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="83" workbookViewId="0">
+      <selection activeCell="J63" sqref="J63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="10" width="48.40625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="48.40625" style="2" customWidth="1"/>
+    <col min="2" max="9" width="17.86328125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="48.40625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="44.25" x14ac:dyDescent="0.75">
@@ -6179,7 +6194,7 @@
         <v>266</v>
       </c>
       <c r="J9" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="409.5" x14ac:dyDescent="0.75">
@@ -7035,7 +7050,7 @@
         <v>292</v>
       </c>
       <c r="J36" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="409.5" x14ac:dyDescent="0.75">
@@ -7271,7 +7286,7 @@
       </c>
       <c r="J44" s="2">
         <f>COUNTIF(J2:J43,TRUE)</f>
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.75">
@@ -7291,7 +7306,7 @@
       </c>
       <c r="J45" s="2">
         <f>COUNTIF(J2:J43,FALSE)</f>
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.75">
@@ -7311,7 +7326,7 @@
       </c>
       <c r="J46" s="2">
         <f>J44/(J44+J45)*100</f>
-        <v>57.499999999999993</v>
+        <v>62.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>